<commit_message>
update BOM for V1.1
</commit_message>
<xml_diff>
--- a/HW/Release/1.1/ZigBug_BOM_V1.1.xlsx
+++ b/HW/Release/1.1/ZigBug_BOM_V1.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="163">
   <si>
     <t>Comment</t>
   </si>
@@ -137,9 +137,6 @@
     <t>0.1u</t>
   </si>
   <si>
-    <t>SchottkyDiode_SOD123</t>
-  </si>
-  <si>
     <t>Diode</t>
   </si>
   <si>
@@ -287,9 +284,6 @@
     <t>R8</t>
   </si>
   <si>
-    <t>5K</t>
-  </si>
-  <si>
     <t>R9</t>
   </si>
   <si>
@@ -515,7 +509,10 @@
     <t>TP5410</t>
   </si>
   <si>
-    <t>5.62K代替</t>
+    <t>SOD123</t>
+  </si>
+  <si>
+    <t>SchottkyDiode</t>
   </si>
 </sst>
 </file>
@@ -870,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -908,7 +905,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="14.65">
@@ -934,7 +931,7 @@
         <v>12</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="14.65">
@@ -1155,115 +1152,115 @@
     </row>
     <row r="12" spans="1:8" ht="14.65">
       <c r="A12" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>161</v>
       </c>
       <c r="F12" s="3">
         <v>2</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="14.65">
       <c r="A13" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="3">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="F13" s="3">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="14.65">
       <c r="A14" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="3">
-        <v>1</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" ht="14.65">
       <c r="A15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="3">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="F15" s="3">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" ht="14.65">
       <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
@@ -1275,43 +1272,43 @@
     </row>
     <row r="17" spans="1:8" ht="14.65">
       <c r="A17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F17" s="3">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8" ht="14.65">
       <c r="A18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="E18" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F18" s="3">
         <v>1</v>
@@ -1320,24 +1317,24 @@
         <v>12</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="14.65">
       <c r="A19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="F19" s="3">
         <v>2</v>
@@ -1345,23 +1342,25 @@
       <c r="G19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="H19" s="2" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="14.65">
       <c r="A20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="E20" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F20" s="3">
         <v>2</v>
@@ -1373,190 +1372,190 @@
     </row>
     <row r="21" spans="1:8" ht="14.65">
       <c r="A21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F21" s="3">
         <v>15</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8" ht="14.65">
       <c r="A22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="C22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="H22" s="2"/>
     </row>
     <row r="23" spans="1:8" ht="14.65">
       <c r="A23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="C23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" ht="14.65">
       <c r="A24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="C24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="3">
-        <v>1</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" ht="14.65">
       <c r="A25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="C25" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F25" s="3">
         <v>1</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>163</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="H25" s="2"/>
     </row>
     <row r="26" spans="1:8" ht="14.65">
       <c r="A26" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>76</v>
-      </c>
       <c r="C26" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F26" s="3">
         <v>1</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H26" s="2"/>
     </row>
     <row r="27" spans="1:8" ht="14.65">
       <c r="A27" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>94</v>
-      </c>
       <c r="F27" s="3">
         <v>1</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H27" s="2"/>
+      <c r="H27" s="2" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="28" spans="1:8" ht="14.65">
       <c r="A28" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="F28" s="3">
         <v>1</v>
       </c>
@@ -1564,24 +1563,24 @@
         <v>12</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="14.65">
       <c r="A29" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
@@ -1590,24 +1589,24 @@
         <v>12</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="14.65">
       <c r="A30" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
@@ -1616,25 +1615,25 @@
         <v>12</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="14.65">
       <c r="A31" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="F31" s="3">
         <v>1</v>
       </c>
@@ -1642,24 +1641,24 @@
         <v>12</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="14.65">
       <c r="A32" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F32" s="3">
         <v>1</v>
@@ -1668,24 +1667,24 @@
         <v>12</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="14.65">
       <c r="A33" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="F33" s="3">
         <v>1</v>
@@ -1697,19 +1696,19 @@
     </row>
     <row r="34" spans="1:8" ht="14.65">
       <c r="A34" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>113</v>
-      </c>
       <c r="E34" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F34" s="3">
         <v>1</v>
@@ -1721,19 +1720,19 @@
     </row>
     <row r="35" spans="1:8" ht="14.65">
       <c r="A35" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F35" s="3">
         <v>1</v>
@@ -1745,19 +1744,19 @@
     </row>
     <row r="36" spans="1:8" ht="14.65">
       <c r="A36" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="E36" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F36" s="3">
         <v>1</v>
@@ -1769,19 +1768,19 @@
     </row>
     <row r="37" spans="1:8" ht="14.65">
       <c r="A37" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>127</v>
-      </c>
       <c r="E37" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F37" s="3">
         <v>4</v>
@@ -1793,19 +1792,19 @@
     </row>
     <row r="38" spans="1:8" ht="14.65">
       <c r="A38" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="E38" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F38" s="3">
         <v>1</v>
@@ -1817,19 +1816,19 @@
     </row>
     <row r="39" spans="1:8" ht="14.65">
       <c r="A39" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>135</v>
       </c>
       <c r="F39" s="3">
         <v>1</v>
@@ -1841,19 +1840,19 @@
     </row>
     <row r="40" spans="1:8" ht="14.65">
       <c r="A40" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>139</v>
-      </c>
       <c r="E40" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F40" s="3">
         <v>1</v>
@@ -1865,19 +1864,19 @@
     </row>
     <row r="41" spans="1:8" ht="14.65">
       <c r="A41" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="D41" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F41" s="3">
         <v>1</v>
@@ -1889,19 +1888,19 @@
     </row>
     <row r="42" spans="1:8" ht="14.65">
       <c r="A42" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="E42" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F42" s="3">
         <v>3</v>
@@ -1913,19 +1912,19 @@
     </row>
     <row r="43" spans="1:8" ht="14.65">
       <c r="A43" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>149</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F43" s="3">
         <v>2</v>
@@ -1937,19 +1936,19 @@
     </row>
     <row r="44" spans="1:8" ht="14.65">
       <c r="A44" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="F44" s="3">
         <v>1</v>
@@ -1961,19 +1960,19 @@
     </row>
     <row r="45" spans="1:8" ht="14.65">
       <c r="A45" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="E45" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F45" s="3">
         <v>1</v>

</xml_diff>